<commit_message>
Added stats JSON and Updated spreadsheet - Push for Mac
</commit_message>
<xml_diff>
--- a/assets/data/Hunt_v2.xlsx
+++ b/assets/data/Hunt_v2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Python\Discord_Bots\doubleLung_Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Python\Discord_Bots\DoubleLung\assets\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D93B0C6-C99E-4E4C-BADC-992E8B8891CB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71F46FBE-7FD0-4CB7-A1D7-6B87508C458B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22800" yWindow="11910" windowWidth="28800" windowHeight="6000" tabRatio="908" activeTab="5" xr2:uid="{49463AEE-7DC0-4014-BA40-AA309B07B9F3}"/>
+    <workbookView xWindow="36840" yWindow="5445" windowWidth="28800" windowHeight="6000" tabRatio="908" activeTab="6" xr2:uid="{49463AEE-7DC0-4014-BA40-AA309B07B9F3}"/>
   </bookViews>
   <sheets>
     <sheet name="Species" sheetId="1" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4626" uniqueCount="1983">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4778" uniqueCount="2037">
   <si>
     <t>active</t>
   </si>
@@ -6003,6 +6003,168 @@
   </si>
   <si>
     <t>["Red Deer","Sika Deer"]</t>
+  </si>
+  <si>
+    <t>speciescommand</t>
+  </si>
+  <si>
+    <t>bighorn</t>
+  </si>
+  <si>
+    <t>blacktail</t>
+  </si>
+  <si>
+    <t>southeastern</t>
+  </si>
+  <si>
+    <t>whitetail</t>
+  </si>
+  <si>
+    <t>wildebeest</t>
+  </si>
+  <si>
+    <t>mouflon</t>
+  </si>
+  <si>
+    <t>wildebeast</t>
+  </si>
+  <si>
+    <t>raindeer</t>
+  </si>
+  <si>
+    <t>rockymountain</t>
+  </si>
+  <si>
+    <t>sidestriped</t>
+  </si>
+  <si>
+    <t>medved</t>
+  </si>
+  <si>
+    <t>silverridge</t>
+  </si>
+  <si>
+    <t>whereabouts</t>
+  </si>
+  <si>
+    <t>sceen</t>
+  </si>
+  <si>
+    <t>setting</t>
+  </si>
+  <si>
+    <t>venue</t>
+  </si>
+  <si>
+    <t>fl</t>
+  </si>
+  <si>
+    <t>07mm</t>
+  </si>
+  <si>
+    <t>7milli</t>
+  </si>
+  <si>
+    <t>07milli</t>
+  </si>
+  <si>
+    <t>7millimeter</t>
+  </si>
+  <si>
+    <t>07millimeter</t>
+  </si>
+  <si>
+    <t>20sa</t>
+  </si>
+  <si>
+    <t>470db</t>
+  </si>
+  <si>
+    <t>3006</t>
+  </si>
+  <si>
+    <t>12guage</t>
+  </si>
+  <si>
+    <t>41045</t>
+  </si>
+  <si>
+    <t>306</t>
+  </si>
+  <si>
+    <t>12g</t>
+  </si>
+  <si>
+    <t>30ought</t>
+  </si>
+  <si>
+    <t>50caliber</t>
+  </si>
+  <si>
+    <t>30ought06</t>
+  </si>
+  <si>
+    <t>30ought6</t>
+  </si>
+  <si>
+    <t>ought06</t>
+  </si>
+  <si>
+    <t>ought6</t>
+  </si>
+  <si>
+    <t>65mm</t>
+  </si>
+  <si>
+    <t>6mm</t>
+  </si>
+  <si>
+    <t>65milli</t>
+  </si>
+  <si>
+    <t>6mili</t>
+  </si>
+  <si>
+    <t>65millimeter</t>
+  </si>
+  <si>
+    <t>6millimeter</t>
+  </si>
+  <si>
+    <t>50cal</t>
+  </si>
+  <si>
+    <t>caplock</t>
+  </si>
+  <si>
+    <t>m1</t>
+  </si>
+  <si>
+    <t>cb165</t>
+  </si>
+  <si>
+    <t>sxs</t>
+  </si>
+  <si>
+    <t>20g</t>
+  </si>
+  <si>
+    <t>20guage</t>
+  </si>
+  <si>
+    <t>cb60</t>
+  </si>
+  <si>
+    <t>hawkedge</t>
+  </si>
+  <si>
+    <t>cb70</t>
+  </si>
+  <si>
+    <t>long</t>
+  </si>
+  <si>
+    <t>6milli</t>
   </si>
 </sst>
 </file>
@@ -6059,12 +6221,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -6080,7 +6248,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -6170,6 +6338,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -11170,53 +11341,50 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CA1C4D7-E97B-4654-9B4A-178195F9AA4A}">
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
-        <v>722</v>
+      <c r="A1" t="s">
+        <v>1983</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="27" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="27" t="s">
         <v>763</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
-        <v>967</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="26" t="s">
+        <v>967</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="26" t="s">
         <v>980</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="27" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="26"/>
-      <c r="C5" s="26"/>
-      <c r="D5" s="26"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="27" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B6" s="26"/>
       <c r="C6" s="26"/>
       <c r="D6" s="26"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="26" t="s">
-        <v>974</v>
+      <c r="A7" s="27" t="s">
+        <v>2</v>
       </c>
       <c r="B7" s="26"/>
       <c r="C7" s="26"/>
@@ -11224,15 +11392,15 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="26" t="s">
-        <v>981</v>
+        <v>974</v>
       </c>
       <c r="B8" s="26"/>
       <c r="C8" s="26"/>
       <c r="D8" s="26"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="27" t="s">
-        <v>3</v>
+      <c r="A9" s="26" t="s">
+        <v>981</v>
       </c>
       <c r="B9" s="26"/>
       <c r="C9" s="26"/>
@@ -11240,114 +11408,122 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="27" t="s">
-        <v>785</v>
+        <v>3</v>
       </c>
       <c r="B10" s="26"/>
       <c r="C10" s="26"/>
       <c r="D10" s="26"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="26" t="s">
-        <v>975</v>
-      </c>
+      <c r="A11" s="27" t="s">
+        <v>785</v>
+      </c>
+      <c r="B11" s="26"/>
+      <c r="C11" s="26"/>
+      <c r="D11" s="26"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="26" t="s">
+        <v>975</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="26" t="s">
         <v>982</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="27" t="s">
-        <v>780</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="27" t="s">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="27" t="s">
         <v>786</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="26" t="s">
-        <v>976</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="26" t="s">
+        <v>976</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="26" t="s">
         <v>816</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="27" t="s">
-        <v>781</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="27" t="s">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="27" t="s">
         <v>957</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="26" t="s">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="26" t="s">
         <v>983</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="27" t="s">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="27" t="s">
         <v>782</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="26" t="s">
-        <v>545</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="26" t="s">
-        <v>977</v>
+        <v>545</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="26" t="s">
+        <v>977</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="26" t="s">
         <v>984</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" s="27" t="s">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="27" t="s">
         <v>783</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" s="26" t="s">
-        <v>771</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="26" t="s">
-        <v>978</v>
+        <v>771</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="26" t="s">
+        <v>978</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="26" t="s">
         <v>985</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" s="27" t="s">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="27" t="s">
         <v>784</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" s="26" t="s">
-        <v>968</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="26" t="s">
-        <v>979</v>
+        <v>968</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="26" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" s="26" t="s">
         <v>986</v>
       </c>
     </row>
@@ -11358,276 +11534,281 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F069AB5-B36F-481D-8674-EDB4DE4D15A4}">
-  <dimension ref="A1:A53"/>
+  <dimension ref="A1:A54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+      <c r="A1" t="s">
+        <v>1983</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="27" t="s">
         <v>787</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="26" t="s">
-        <v>814</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
-        <v>813</v>
+        <v>814</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="26" t="s">
-        <v>1004</v>
+        <v>813</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="26" t="s">
+        <v>1004</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="26" t="s">
         <v>817</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="27" t="s">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="27" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="26" t="s">
-        <v>958</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="26" t="s">
-        <v>993</v>
+        <v>958</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="26" t="s">
-        <v>788</v>
+        <v>993</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="26" t="s">
-        <v>815</v>
+        <v>788</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="26" t="s">
-        <v>959</v>
+        <v>815</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="26" t="s">
-        <v>994</v>
+        <v>959</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="26" t="s">
-        <v>1005</v>
+        <v>994</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="26" t="s">
+        <v>1005</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" s="26" t="s">
         <v>1015</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" s="27" t="s">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" s="27" t="s">
         <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" s="26" t="s">
-        <v>960</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="26" t="s">
-        <v>995</v>
+        <v>960</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="26" t="s">
-        <v>1006</v>
+        <v>995</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="26" t="s">
+        <v>1006</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="26" t="s">
         <v>1016</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="27" t="s">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="27" t="s">
         <v>764</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="26" t="s">
-        <v>961</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="26" t="s">
-        <v>996</v>
+        <v>961</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="26" t="s">
-        <v>1007</v>
+        <v>996</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="26" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="26" t="s">
         <v>1017</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" s="27" t="s">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="27" t="s">
         <v>789</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" s="26" t="s">
-        <v>962</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="26" t="s">
-        <v>790</v>
+        <v>962</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="26" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="26" t="s">
         <v>1008</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" s="27" t="s">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" s="27" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" s="26" t="s">
-        <v>779</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="26" t="s">
-        <v>997</v>
+        <v>779</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="26" t="s">
+        <v>997</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="26" t="s">
         <v>1009</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="27" t="s">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="27" t="s">
         <v>763</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="26" t="s">
-        <v>998</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="26" t="s">
-        <v>1010</v>
+        <v>998</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="26" t="s">
-        <v>767</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="26" t="s">
-        <v>999</v>
+        <v>767</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="26" t="s">
+        <v>999</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" s="26" t="s">
         <v>1011</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" s="27" t="s">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" s="27" t="s">
         <v>791</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" s="26" t="s">
-        <v>964</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="26" t="s">
-        <v>1000</v>
+        <v>964</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="26" t="s">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" s="26" t="s">
         <v>1012</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43" s="27" t="s">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" s="27" t="s">
         <v>792</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A44" s="26" t="s">
-        <v>965</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" s="26" t="s">
-        <v>1001</v>
+        <v>965</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" s="26" t="s">
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" s="26" t="s">
         <v>1013</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A47" s="27" t="s">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" s="27" t="s">
         <v>716</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A48" s="26" t="s">
-        <v>963</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="26" t="s">
-        <v>1002</v>
+        <v>963</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="26" t="s">
+        <v>1002</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" s="26" t="s">
         <v>1014</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A51" s="27" t="s">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" s="27" t="s">
         <v>793</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52" s="26" t="s">
-        <v>336</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" s="26" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" s="26" t="s">
         <v>1003</v>
       </c>
     </row>
@@ -11638,164 +11819,167 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81F0560E-3944-427C-8950-2A67E8822FAD}">
-  <dimension ref="A1:AW96"/>
+  <dimension ref="A1:AX96"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="R66" sqref="R66"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+    <row r="1" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1983</v>
+      </c>
+      <c r="B1" s="27" t="s">
         <v>794</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="C1" s="27" t="s">
         <v>795</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="D1" s="27" t="s">
         <v>796</v>
       </c>
-      <c r="D1" s="27" t="s">
+      <c r="E1" s="27" t="s">
         <v>797</v>
       </c>
-      <c r="E1" s="27" t="s">
+      <c r="F1" s="27" t="s">
         <v>724</v>
       </c>
-      <c r="F1" s="27" t="s">
+      <c r="G1" s="27" t="s">
         <v>798</v>
       </c>
-      <c r="G1" s="27" t="s">
+      <c r="H1" s="27" t="s">
         <v>342</v>
       </c>
-      <c r="H1" s="27" t="s">
+      <c r="I1" s="27" t="s">
         <v>799</v>
       </c>
-      <c r="I1" s="27" t="s">
+      <c r="J1" s="27" t="s">
         <v>800</v>
       </c>
-      <c r="J1" s="27" t="s">
+      <c r="K1" s="27" t="s">
         <v>801</v>
       </c>
-      <c r="K1" s="27" t="s">
+      <c r="L1" s="27" t="s">
         <v>802</v>
       </c>
-      <c r="L1" s="27" t="s">
+      <c r="M1" s="27" t="s">
         <v>803</v>
       </c>
-      <c r="M1" s="27" t="s">
+      <c r="N1" s="27" t="s">
         <v>804</v>
       </c>
-      <c r="N1" s="27" t="s">
+      <c r="O1" s="27" t="s">
         <v>805</v>
       </c>
-      <c r="O1" s="27" t="s">
+      <c r="P1" s="27" t="s">
         <v>806</v>
       </c>
-      <c r="P1" s="27" t="s">
+      <c r="Q1" s="27" t="s">
         <v>807</v>
       </c>
-      <c r="Q1" s="27" t="s">
+      <c r="R1" s="27" t="s">
         <v>808</v>
       </c>
-      <c r="R1" s="27" t="s">
+      <c r="S1" s="27" t="s">
         <v>809</v>
       </c>
-      <c r="S1" s="27" t="s">
+      <c r="T1" s="27" t="s">
         <v>588</v>
       </c>
-      <c r="T1" s="26" t="s">
+      <c r="U1" s="26" t="s">
         <v>589</v>
       </c>
-      <c r="U1" s="26" t="s">
+      <c r="V1" s="26" t="s">
         <v>1038</v>
       </c>
-      <c r="V1" s="26" t="s">
+      <c r="W1" s="26" t="s">
         <v>1039</v>
       </c>
-      <c r="W1" s="26" t="s">
+      <c r="X1" s="26" t="s">
         <v>1018</v>
       </c>
-      <c r="X1" s="26" t="s">
+      <c r="Y1" s="26" t="s">
         <v>1019</v>
       </c>
-      <c r="Y1" s="26" t="s">
+      <c r="Z1" s="26" t="s">
         <v>1020</v>
       </c>
-      <c r="Z1" s="26" t="s">
+      <c r="AA1" s="26" t="s">
         <v>1021</v>
       </c>
-      <c r="AA1" s="26" t="s">
+      <c r="AB1" s="26" t="s">
         <v>1022</v>
       </c>
-      <c r="AB1" s="26" t="s">
+      <c r="AC1" s="26" t="s">
         <v>1023</v>
       </c>
-      <c r="AC1" s="26" t="s">
+      <c r="AD1" s="26" t="s">
         <v>1024</v>
       </c>
-      <c r="AD1" s="26" t="s">
+      <c r="AE1" s="26" t="s">
         <v>754</v>
       </c>
-      <c r="AE1" s="26" t="s">
+      <c r="AF1" s="26" t="s">
         <v>1025</v>
       </c>
-      <c r="AF1" s="26" t="s">
+      <c r="AG1" s="26" t="s">
         <v>1026</v>
       </c>
-      <c r="AG1" s="26" t="s">
+      <c r="AH1" s="26" t="s">
         <v>1027</v>
       </c>
-      <c r="AH1" s="26" t="s">
+      <c r="AI1" s="26" t="s">
         <v>1028</v>
       </c>
-      <c r="AI1" s="26" t="s">
+      <c r="AJ1" s="26" t="s">
         <v>1029</v>
       </c>
-      <c r="AJ1" s="26" t="s">
+      <c r="AK1" s="26" t="s">
         <v>800</v>
       </c>
-      <c r="AK1" s="26" t="s">
+      <c r="AL1" s="26" t="s">
         <v>803</v>
       </c>
-      <c r="AL1" s="26" t="s">
+      <c r="AM1" s="26" t="s">
         <v>1030</v>
       </c>
-      <c r="AM1" s="26" t="s">
+      <c r="AN1" s="26" t="s">
         <v>804</v>
       </c>
-      <c r="AN1" s="26" t="s">
+      <c r="AO1" s="26" t="s">
         <v>807</v>
       </c>
-      <c r="AO1" s="26" t="s">
+      <c r="AP1" s="26" t="s">
         <v>800</v>
       </c>
-      <c r="AP1" s="26" t="s">
+      <c r="AQ1" s="26" t="s">
         <v>1031</v>
       </c>
-      <c r="AQ1" s="26" t="s">
+      <c r="AR1" s="26" t="s">
         <v>1032</v>
       </c>
-      <c r="AR1" s="26" t="s">
+      <c r="AS1" s="26" t="s">
         <v>1033</v>
       </c>
-      <c r="AS1" s="26" t="s">
+      <c r="AT1" s="26" t="s">
         <v>807</v>
       </c>
-      <c r="AT1" s="26" t="s">
+      <c r="AU1" s="26" t="s">
         <v>1034</v>
       </c>
-      <c r="AU1" s="26" t="s">
+      <c r="AV1" s="26" t="s">
         <v>1035</v>
       </c>
-      <c r="AV1" s="26" t="s">
+      <c r="AW1" s="26" t="s">
         <v>1036</v>
       </c>
-      <c r="AW1" s="26" t="s">
+      <c r="AX1" s="26" t="s">
         <v>1037</v>
       </c>
     </row>
-    <row r="2" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>880</v>
       </c>
@@ -11806,7 +11990,7 @@
       <c r="D2" s="18"/>
       <c r="E2" s="18"/>
     </row>
-    <row r="3" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>939</v>
       </c>
@@ -11817,7 +12001,7 @@
       <c r="D3" s="18"/>
       <c r="E3" s="18"/>
     </row>
-    <row r="4" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
         <v>940</v>
       </c>
@@ -11828,7 +12012,7 @@
       <c r="D4" s="18"/>
       <c r="E4" s="18"/>
     </row>
-    <row r="5" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
         <v>941</v>
       </c>
@@ -11839,7 +12023,7 @@
       <c r="D5" s="18"/>
       <c r="E5" s="18"/>
     </row>
-    <row r="6" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
         <v>849</v>
       </c>
@@ -11856,7 +12040,7 @@
         <v>853</v>
       </c>
     </row>
-    <row r="7" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
         <v>726</v>
       </c>
@@ -11873,7 +12057,7 @@
         <v>853</v>
       </c>
     </row>
-    <row r="8" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
         <v>942</v>
       </c>
@@ -11884,7 +12068,7 @@
       <c r="D8" s="18"/>
       <c r="E8" s="18"/>
     </row>
-    <row r="9" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
         <v>943</v>
       </c>
@@ -11895,7 +12079,7 @@
       <c r="D9" s="18"/>
       <c r="E9" s="18"/>
     </row>
-    <row r="10" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
         <v>887</v>
       </c>
@@ -11906,7 +12090,7 @@
       <c r="D10" s="18"/>
       <c r="E10" s="18"/>
     </row>
-    <row r="11" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A11" s="18" t="s">
         <v>945</v>
       </c>
@@ -11917,7 +12101,7 @@
       <c r="D11" s="18"/>
       <c r="E11" s="18"/>
     </row>
-    <row r="12" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
         <v>884</v>
       </c>
@@ -11930,7 +12114,7 @@
       <c r="D12" s="18"/>
       <c r="E12" s="18"/>
     </row>
-    <row r="13" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
         <v>947</v>
       </c>
@@ -11945,7 +12129,7 @@
       </c>
       <c r="E13" s="18"/>
     </row>
-    <row r="14" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
         <v>887</v>
       </c>
@@ -11960,7 +12144,7 @@
       </c>
       <c r="E14" s="18"/>
     </row>
-    <row r="15" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
         <v>949</v>
       </c>
@@ -11975,7 +12159,7 @@
       </c>
       <c r="E15" s="18"/>
     </row>
-    <row r="16" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A16" s="18" t="s">
         <v>950</v>
       </c>
@@ -13444,7 +13628,7 @@
   <dimension ref="A1:P37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:H37"/>
+      <selection sqref="A1:P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14165,7 +14349,7 @@
   <dimension ref="A1:Q33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E33"/>
+      <selection sqref="A1:Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14631,7 +14815,7 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C10"/>
+      <selection sqref="A1:I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14758,7 +14942,7 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18333,7 +18517,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C10FC8FB-6680-A940-A410-8E355950D6A9}">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
@@ -18557,8 +18741,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BAD2FA7-52EE-4B9F-95EA-395442F103BB}">
   <dimension ref="A1:BK235"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" topLeftCell="A86" workbookViewId="0">
+      <selection activeCell="A116" sqref="A116:XFD116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -18732,7 +18916,9 @@
       <c r="D4" s="27" t="s">
         <v>723</v>
       </c>
-      <c r="E4" s="27"/>
+      <c r="E4" s="27" t="s">
+        <v>1984</v>
+      </c>
       <c r="F4" s="27"/>
       <c r="G4" s="27"/>
       <c r="H4" s="27"/>
@@ -18773,7 +18959,9 @@
       <c r="C6" s="27" t="s">
         <v>724</v>
       </c>
-      <c r="D6" s="27"/>
+      <c r="D6" s="27" t="s">
+        <v>91</v>
+      </c>
       <c r="E6" s="27"/>
       <c r="F6" s="27"/>
       <c r="G6" s="27"/>
@@ -18797,7 +18985,9 @@
       <c r="D7" s="27" t="s">
         <v>653</v>
       </c>
-      <c r="E7" s="27"/>
+      <c r="E7" s="27" t="s">
+        <v>1985</v>
+      </c>
       <c r="F7" s="27"/>
       <c r="G7" s="27"/>
       <c r="H7" s="27"/>
@@ -18826,8 +19016,12 @@
       <c r="F8" s="27" t="s">
         <v>718</v>
       </c>
-      <c r="G8" s="27"/>
-      <c r="H8" s="27"/>
+      <c r="G8" s="27" t="s">
+        <v>1988</v>
+      </c>
+      <c r="H8" s="27" t="s">
+        <v>1990</v>
+      </c>
       <c r="I8" s="27"/>
       <c r="J8" s="27"/>
       <c r="K8" s="27"/>
@@ -18844,8 +19038,12 @@
       <c r="C9" s="27" t="s">
         <v>665</v>
       </c>
-      <c r="D9" s="27"/>
-      <c r="E9" s="27"/>
+      <c r="D9" s="27" t="s">
+        <v>663</v>
+      </c>
+      <c r="E9" s="27" t="s">
+        <v>666</v>
+      </c>
       <c r="F9" s="27"/>
       <c r="G9" s="27"/>
       <c r="H9" s="27"/>
@@ -19146,7 +19344,9 @@
       <c r="C23" s="27" t="s">
         <v>677</v>
       </c>
-      <c r="D23" s="27"/>
+      <c r="D23" s="27" t="s">
+        <v>108</v>
+      </c>
       <c r="E23" s="27"/>
       <c r="F23" s="27"/>
       <c r="G23" s="27"/>
@@ -19268,7 +19468,9 @@
       <c r="D28" s="27" t="s">
         <v>688</v>
       </c>
-      <c r="E28" s="27"/>
+      <c r="E28" s="27" t="s">
+        <v>1989</v>
+      </c>
       <c r="F28" s="27"/>
       <c r="G28" s="27"/>
       <c r="H28" s="27"/>
@@ -19311,7 +19513,9 @@
       <c r="C30" s="27" t="s">
         <v>671</v>
       </c>
-      <c r="D30" s="27"/>
+      <c r="D30" s="27" t="s">
+        <v>115</v>
+      </c>
       <c r="E30" s="27"/>
       <c r="F30" s="27"/>
       <c r="G30" s="27"/>
@@ -19517,7 +19721,9 @@
       <c r="C40" s="27" t="s">
         <v>697</v>
       </c>
-      <c r="D40" s="27"/>
+      <c r="D40" s="27" t="s">
+        <v>124</v>
+      </c>
       <c r="E40" s="27"/>
       <c r="F40" s="27"/>
       <c r="G40" s="27"/>
@@ -19557,7 +19763,9 @@
       <c r="C42" s="27" t="s">
         <v>653</v>
       </c>
-      <c r="D42" s="27"/>
+      <c r="D42" s="27" t="s">
+        <v>126</v>
+      </c>
       <c r="E42" s="27"/>
       <c r="F42" s="27"/>
       <c r="G42" s="27"/>
@@ -19602,8 +19810,12 @@
       <c r="D44" s="27" t="s">
         <v>873</v>
       </c>
-      <c r="E44" s="27"/>
-      <c r="F44" s="27"/>
+      <c r="E44" s="27" t="s">
+        <v>128</v>
+      </c>
+      <c r="F44" s="27" t="s">
+        <v>1991</v>
+      </c>
       <c r="G44" s="27"/>
       <c r="H44" s="27"/>
       <c r="I44" s="27"/>
@@ -19625,7 +19837,9 @@
       <c r="D45" s="27" t="s">
         <v>568</v>
       </c>
-      <c r="E45" s="27"/>
+      <c r="E45" s="27" t="s">
+        <v>1992</v>
+      </c>
       <c r="F45" s="27"/>
       <c r="G45" s="27"/>
       <c r="H45" s="27"/>
@@ -19645,7 +19859,9 @@
       <c r="C46" s="27" t="s">
         <v>653</v>
       </c>
-      <c r="D46" s="27"/>
+      <c r="D46" s="27" t="s">
+        <v>130</v>
+      </c>
       <c r="E46" s="27"/>
       <c r="F46" s="27"/>
       <c r="G46" s="27"/>
@@ -19708,7 +19924,9 @@
       <c r="C49" s="27" t="s">
         <v>670</v>
       </c>
-      <c r="D49" s="27"/>
+      <c r="D49" s="27" t="s">
+        <v>133</v>
+      </c>
       <c r="E49" s="27"/>
       <c r="F49" s="27"/>
       <c r="G49" s="27"/>
@@ -19732,7 +19950,9 @@
       <c r="D50" s="27" t="s">
         <v>709</v>
       </c>
-      <c r="E50" s="27"/>
+      <c r="E50" s="27" t="s">
+        <v>1993</v>
+      </c>
       <c r="F50" s="27"/>
       <c r="G50" s="27"/>
       <c r="H50" s="27"/>
@@ -19775,7 +19995,9 @@
       <c r="D52" s="27" t="s">
         <v>681</v>
       </c>
-      <c r="E52" s="27"/>
+      <c r="E52" s="27" t="s">
+        <v>1986</v>
+      </c>
       <c r="F52" s="27"/>
       <c r="G52" s="27"/>
       <c r="H52" s="27"/>
@@ -19795,7 +20017,9 @@
       <c r="C53" s="27" t="s">
         <v>677</v>
       </c>
-      <c r="D53" s="27"/>
+      <c r="D53" s="27" t="s">
+        <v>138</v>
+      </c>
       <c r="E53" s="27"/>
       <c r="F53" s="27"/>
       <c r="G53" s="27"/>
@@ -19835,7 +20059,9 @@
       <c r="C55" s="27" t="s">
         <v>715</v>
       </c>
-      <c r="D55" s="27"/>
+      <c r="D55" s="27" t="s">
+        <v>140</v>
+      </c>
       <c r="E55" s="27"/>
       <c r="F55" s="27"/>
       <c r="G55" s="27"/>
@@ -19880,7 +20106,9 @@
       <c r="D57" s="27" t="s">
         <v>653</v>
       </c>
-      <c r="E57" s="27"/>
+      <c r="E57" s="27" t="s">
+        <v>1987</v>
+      </c>
       <c r="F57" s="27"/>
       <c r="G57" s="27"/>
       <c r="H57" s="27"/>
@@ -19915,6 +20143,39 @@
       <c r="A60" s="21" t="s">
         <v>595</v>
       </c>
+      <c r="B60" s="26" t="s">
+        <v>336</v>
+      </c>
+      <c r="C60" s="26" t="s">
+        <v>958</v>
+      </c>
+      <c r="D60" s="26" t="s">
+        <v>959</v>
+      </c>
+      <c r="E60" s="26" t="s">
+        <v>961</v>
+      </c>
+      <c r="F60" s="26" t="s">
+        <v>962</v>
+      </c>
+      <c r="G60" s="26" t="s">
+        <v>1996</v>
+      </c>
+      <c r="H60" s="26" t="s">
+        <v>1997</v>
+      </c>
+      <c r="I60" s="26" t="s">
+        <v>1998</v>
+      </c>
+      <c r="J60" s="26" t="s">
+        <v>767</v>
+      </c>
+      <c r="K60" s="26" t="s">
+        <v>964</v>
+      </c>
+      <c r="L60" s="26" t="s">
+        <v>1999</v>
+      </c>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A61" s="22" t="s">
@@ -19926,6 +20187,9 @@
       <c r="C61" s="26" t="s">
         <v>736</v>
       </c>
+      <c r="D61" s="26" t="s">
+        <v>578</v>
+      </c>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A62" s="22" t="s">
@@ -19951,6 +20215,9 @@
       <c r="D63" s="26" t="s">
         <v>739</v>
       </c>
+      <c r="E63" s="26" t="s">
+        <v>1994</v>
+      </c>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A64" s="22" t="s">
@@ -19963,7 +20230,7 @@
         <v>744</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A65" s="22" t="s">
         <v>55</v>
       </c>
@@ -19974,7 +20241,7 @@
         <v>740</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A66" s="22" t="s">
         <v>61</v>
       </c>
@@ -19985,7 +20252,7 @@
         <v>746</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A67" s="22" t="s">
         <v>69</v>
       </c>
@@ -19999,7 +20266,7 @@
         <v>748</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A68" s="22" t="s">
         <v>76</v>
       </c>
@@ -20015,8 +20282,11 @@
       <c r="E68" s="26" t="s">
         <v>876</v>
       </c>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F68" s="26" t="s">
+        <v>1995</v>
+      </c>
+    </row>
+    <row r="69" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A69" s="22" t="s">
         <v>81</v>
       </c>
@@ -20027,12 +20297,60 @@
         <v>751</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A71" s="22" t="s">
         <v>596</v>
       </c>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B71" s="18" t="s">
+        <v>1029</v>
+      </c>
+      <c r="C71" s="18" t="s">
+        <v>800</v>
+      </c>
+      <c r="D71" s="18" t="s">
+        <v>803</v>
+      </c>
+      <c r="E71" s="18" t="s">
+        <v>1030</v>
+      </c>
+      <c r="F71" s="18" t="s">
+        <v>804</v>
+      </c>
+      <c r="G71" s="18" t="s">
+        <v>807</v>
+      </c>
+      <c r="H71" s="18" t="s">
+        <v>800</v>
+      </c>
+      <c r="I71" s="18" t="s">
+        <v>588</v>
+      </c>
+      <c r="J71" s="18" t="s">
+        <v>806</v>
+      </c>
+      <c r="K71" s="18" t="s">
+        <v>1047</v>
+      </c>
+      <c r="L71" s="18" t="s">
+        <v>802</v>
+      </c>
+      <c r="M71" s="18" t="s">
+        <v>1048</v>
+      </c>
+      <c r="N71" s="18" t="s">
+        <v>1049</v>
+      </c>
+      <c r="O71" s="18" t="s">
+        <v>1000</v>
+      </c>
+      <c r="P71" s="18" t="s">
+        <v>1050</v>
+      </c>
+      <c r="Q71" s="18" t="s">
+        <v>1051</v>
+      </c>
+    </row>
+    <row r="72" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A72" s="28" t="s">
         <v>600</v>
       </c>
@@ -20043,7 +20361,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A73" s="28" t="s">
         <v>601</v>
       </c>
@@ -20054,7 +20372,7 @@
         <v>878</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A74" s="28" t="s">
         <v>602</v>
       </c>
@@ -20068,7 +20386,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A75" s="28" t="s">
         <v>603</v>
       </c>
@@ -20081,8 +20399,11 @@
       <c r="D75" s="26" t="s">
         <v>886</v>
       </c>
-    </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="E75" s="26" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="76" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A76" s="28" t="s">
         <v>604</v>
       </c>
@@ -20110,8 +20431,26 @@
       <c r="I76" s="26" t="s">
         <v>728</v>
       </c>
-    </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J76" s="26" t="s">
+        <v>378</v>
+      </c>
+      <c r="K76" s="26" t="s">
+        <v>2001</v>
+      </c>
+      <c r="L76" s="26" t="s">
+        <v>2002</v>
+      </c>
+      <c r="M76" s="26" t="s">
+        <v>2003</v>
+      </c>
+      <c r="N76" s="26" t="s">
+        <v>2004</v>
+      </c>
+      <c r="O76" s="26" t="s">
+        <v>2005</v>
+      </c>
+    </row>
+    <row r="77" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A77" s="28" t="s">
         <v>605</v>
       </c>
@@ -20124,8 +20463,11 @@
       <c r="D77" s="26" t="s">
         <v>879</v>
       </c>
-    </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="E77" s="26" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="78" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A78" s="28" t="s">
         <v>606</v>
       </c>
@@ -20141,8 +20483,11 @@
       <c r="E78" s="26" t="s">
         <v>731</v>
       </c>
-    </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F78" s="26" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="79" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A79" s="28" t="s">
         <v>607</v>
       </c>
@@ -20161,8 +20506,14 @@
       <c r="F79" s="26" t="s">
         <v>889</v>
       </c>
-    </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G79" s="26" t="s">
+        <v>471</v>
+      </c>
+      <c r="H79" s="26" t="s">
+        <v>946</v>
+      </c>
+    </row>
+    <row r="80" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A80" s="28" t="s">
         <v>608</v>
       </c>
@@ -20175,8 +20526,11 @@
       <c r="D80" s="26" t="s">
         <v>832</v>
       </c>
-    </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="E80" s="26" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="81" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A81" s="28" t="s">
         <v>609</v>
       </c>
@@ -20190,10 +20544,13 @@
         <v>839</v>
       </c>
       <c r="E81" s="26" t="s">
+        <v>2007</v>
+      </c>
+      <c r="F81" s="26" t="s">
         <v>833</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A82" s="28" t="s">
         <v>610</v>
       </c>
@@ -20213,7 +20570,7 @@
         <v>830</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A83" s="28" t="s">
         <v>611</v>
       </c>
@@ -20230,7 +20587,7 @@
         <v>728</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A84" s="28" t="s">
         <v>612</v>
       </c>
@@ -20244,7 +20601,7 @@
         <v>884</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A85" s="28" t="s">
         <v>613</v>
       </c>
@@ -20263,8 +20620,29 @@
       <c r="F85" s="26" t="s">
         <v>850</v>
       </c>
-    </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G85" s="26" t="s">
+        <v>2008</v>
+      </c>
+      <c r="H85" s="26" t="s">
+        <v>2011</v>
+      </c>
+      <c r="I85" s="26" t="s">
+        <v>2013</v>
+      </c>
+      <c r="J85" s="26" t="s">
+        <v>2015</v>
+      </c>
+      <c r="K85" s="26" t="s">
+        <v>2016</v>
+      </c>
+      <c r="L85" s="26" t="s">
+        <v>2017</v>
+      </c>
+      <c r="M85" s="26" t="s">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="86" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A86" s="28" t="s">
         <v>614</v>
       </c>
@@ -20292,8 +20670,26 @@
       <c r="I86" s="26" t="s">
         <v>853</v>
       </c>
-    </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J86" s="26" t="s">
+        <v>2019</v>
+      </c>
+      <c r="K86" s="26" t="s">
+        <v>2020</v>
+      </c>
+      <c r="L86" s="26" t="s">
+        <v>2021</v>
+      </c>
+      <c r="M86" s="26" t="s">
+        <v>2022</v>
+      </c>
+      <c r="N86" s="26" t="s">
+        <v>2023</v>
+      </c>
+      <c r="O86" s="26" t="s">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="87" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A87" s="28" t="s">
         <v>615</v>
       </c>
@@ -20315,8 +20711,17 @@
       <c r="G87" s="26" t="s">
         <v>857</v>
       </c>
-    </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H87" s="26" t="s">
+        <v>2025</v>
+      </c>
+      <c r="I87" s="26" t="s">
+        <v>2014</v>
+      </c>
+      <c r="J87" s="26" t="s">
+        <v>2026</v>
+      </c>
+    </row>
+    <row r="88" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A88" s="28" t="s">
         <v>616</v>
       </c>
@@ -20332,8 +20737,11 @@
       <c r="E88" s="26" t="s">
         <v>902</v>
       </c>
-    </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F88" s="26" t="s">
+        <v>2027</v>
+      </c>
+    </row>
+    <row r="89" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A89" s="28" t="s">
         <v>617</v>
       </c>
@@ -20352,8 +20760,11 @@
       <c r="F89" s="26" t="s">
         <v>895</v>
       </c>
-    </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G89" s="26" t="s">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="90" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A90" s="28" t="s">
         <v>618</v>
       </c>
@@ -20375,8 +20786,17 @@
       <c r="G90" s="26" t="s">
         <v>875</v>
       </c>
-    </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H90" s="26" t="s">
+        <v>482</v>
+      </c>
+      <c r="I90" s="26" t="s">
+        <v>2012</v>
+      </c>
+      <c r="J90" s="26" t="s">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="91" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A91" s="28" t="s">
         <v>619</v>
       </c>
@@ -20392,8 +20812,14 @@
       <c r="E91" s="26" t="s">
         <v>875</v>
       </c>
-    </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F91" s="26" t="s">
+        <v>2012</v>
+      </c>
+      <c r="G91" s="26" t="s">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="92" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A92" s="28" t="s">
         <v>620</v>
       </c>
@@ -20418,8 +20844,17 @@
       <c r="H92" s="26" t="s">
         <v>875</v>
       </c>
-    </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I92" s="26" t="s">
+        <v>2029</v>
+      </c>
+      <c r="J92" s="26" t="s">
+        <v>2030</v>
+      </c>
+      <c r="K92" s="26" t="s">
+        <v>2031</v>
+      </c>
+    </row>
+    <row r="93" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A93" s="28" t="s">
         <v>621</v>
       </c>
@@ -20432,8 +20867,11 @@
       <c r="D93" s="26" t="s">
         <v>891</v>
       </c>
-    </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="E93" s="26" t="s">
+        <v>2006</v>
+      </c>
+    </row>
+    <row r="94" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A94" s="28" t="s">
         <v>622</v>
       </c>
@@ -20447,7 +20885,7 @@
         <v>804</v>
       </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A95" s="28" t="s">
         <v>623</v>
       </c>
@@ -20461,7 +20899,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A96" s="28" t="s">
         <v>624</v>
       </c>
@@ -20474,8 +20912,11 @@
       <c r="D96" s="26" t="s">
         <v>800</v>
       </c>
-    </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E96" s="26" t="s">
+        <v>808</v>
+      </c>
+    </row>
+    <row r="97" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A97" s="28" t="s">
         <v>625</v>
       </c>
@@ -20486,7 +20927,7 @@
         <v>897</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A98" s="28" t="s">
         <v>626</v>
       </c>
@@ -20503,7 +20944,7 @@
         <v>728</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A99" s="28" t="s">
         <v>627</v>
       </c>
@@ -20514,7 +20955,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A100" s="28" t="s">
         <v>628</v>
       </c>
@@ -20533,8 +20974,11 @@
       <c r="F100" s="26" t="s">
         <v>918</v>
       </c>
-    </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G100" s="26" t="s">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="101" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A101" s="28" t="s">
         <v>629</v>
       </c>
@@ -20547,8 +20991,11 @@
       <c r="D101" s="26" t="s">
         <v>832</v>
       </c>
-    </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E101" s="26" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="102" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A102" s="28" t="s">
         <v>630</v>
       </c>
@@ -20564,8 +21011,14 @@
       <c r="E102" s="26" t="s">
         <v>899</v>
       </c>
-    </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F102" s="26" t="s">
+        <v>494</v>
+      </c>
+      <c r="G102" s="26" t="s">
+        <v>2028</v>
+      </c>
+    </row>
+    <row r="103" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A103" s="28" t="s">
         <v>631</v>
       </c>
@@ -20587,8 +21040,14 @@
       <c r="G103" s="26" t="s">
         <v>900</v>
       </c>
-    </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H103" s="26" t="s">
+        <v>495</v>
+      </c>
+      <c r="I103" s="26" t="s">
+        <v>2032</v>
+      </c>
+    </row>
+    <row r="104" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A104" s="28" t="s">
         <v>632</v>
       </c>
@@ -20610,8 +21069,14 @@
       <c r="G104" s="26" t="s">
         <v>900</v>
       </c>
-    </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H104" s="26" t="s">
+        <v>496</v>
+      </c>
+      <c r="I104" s="26" t="s">
+        <v>2032</v>
+      </c>
+    </row>
+    <row r="105" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A105" s="28" t="s">
         <v>633</v>
       </c>
@@ -20625,7 +21090,7 @@
         <v>797</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A106" s="28" t="s">
         <v>634</v>
       </c>
@@ -20641,8 +21106,14 @@
       <c r="E106" s="26" t="s">
         <v>889</v>
       </c>
-    </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F106" s="26" t="s">
+        <v>2033</v>
+      </c>
+      <c r="G106" s="26" t="s">
+        <v>2034</v>
+      </c>
+    </row>
+    <row r="107" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A107" s="23" t="s">
         <v>635</v>
       </c>
@@ -20655,13 +21126,70 @@
       <c r="D107" s="26" t="s">
         <v>894</v>
       </c>
-    </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E107" s="26" t="s">
+        <v>2035</v>
+      </c>
+      <c r="F107" s="26" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="109" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A109" s="28" t="s">
         <v>597</v>
       </c>
-    </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B109" s="18" t="s">
+        <v>1031</v>
+      </c>
+      <c r="C109" s="18" t="s">
+        <v>1032</v>
+      </c>
+      <c r="D109" s="18" t="s">
+        <v>1033</v>
+      </c>
+      <c r="E109" s="18" t="s">
+        <v>807</v>
+      </c>
+      <c r="F109" s="18" t="s">
+        <v>1034</v>
+      </c>
+      <c r="G109" s="18" t="s">
+        <v>1035</v>
+      </c>
+      <c r="H109" s="18" t="s">
+        <v>1036</v>
+      </c>
+      <c r="I109" s="18" t="s">
+        <v>1037</v>
+      </c>
+      <c r="J109" s="18" t="s">
+        <v>589</v>
+      </c>
+      <c r="K109" s="18" t="s">
+        <v>806</v>
+      </c>
+      <c r="L109" s="18" t="s">
+        <v>1047</v>
+      </c>
+      <c r="M109" s="18" t="s">
+        <v>802</v>
+      </c>
+      <c r="N109" s="18" t="s">
+        <v>1048</v>
+      </c>
+      <c r="O109" s="18" t="s">
+        <v>1049</v>
+      </c>
+      <c r="P109" s="18" t="s">
+        <v>1000</v>
+      </c>
+      <c r="Q109" s="18" t="s">
+        <v>1050</v>
+      </c>
+      <c r="R109" s="18" t="s">
+        <v>1051</v>
+      </c>
+    </row>
+    <row r="110" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A110" s="26" t="s">
         <v>636</v>
       </c>
@@ -20671,8 +21199,11 @@
       <c r="C110" s="26" t="s">
         <v>832</v>
       </c>
-    </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D110" s="26" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="111" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A111" s="26">
         <v>0.223</v>
       </c>
@@ -20683,7 +21214,7 @@
         <v>877</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A112" s="26">
         <v>0.24299999999999999</v>
       </c>
@@ -20724,6 +21255,24 @@
       <c r="F114" s="26" t="s">
         <v>853</v>
       </c>
+      <c r="G114" s="26" t="s">
+        <v>2020</v>
+      </c>
+      <c r="H114" s="26" t="s">
+        <v>2019</v>
+      </c>
+      <c r="I114" s="26" t="s">
+        <v>2036</v>
+      </c>
+      <c r="J114" s="26" t="s">
+        <v>2021</v>
+      </c>
+      <c r="K114" s="26" t="s">
+        <v>2024</v>
+      </c>
+      <c r="L114" s="26" t="s">
+        <v>2023</v>
+      </c>
     </row>
     <row r="115" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A115" s="26" t="s">
@@ -20744,16 +21293,34 @@
       <c r="F115" s="26" t="s">
         <v>853</v>
       </c>
+      <c r="G115" s="26" t="s">
+        <v>378</v>
+      </c>
+      <c r="H115" s="26" t="s">
+        <v>2001</v>
+      </c>
+      <c r="I115" s="26" t="s">
+        <v>2002</v>
+      </c>
+      <c r="J115" s="26" t="s">
+        <v>2003</v>
+      </c>
+      <c r="K115" s="26" t="s">
+        <v>2004</v>
+      </c>
+      <c r="L115" s="26" t="s">
+        <v>2005</v>
+      </c>
       <c r="M115" s="27"/>
     </row>
-    <row r="116" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A116" s="26">
+    <row r="116" spans="1:13" s="37" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A116" s="37">
         <v>0.33800000000000002</v>
       </c>
-      <c r="B116" s="26" t="s">
+      <c r="B116" s="37" t="s">
         <v>942</v>
       </c>
-      <c r="C116" s="26" t="s">
+      <c r="C116" s="37" t="s">
         <v>879</v>
       </c>
     </row>
@@ -21090,8 +21657,18 @@
       <c r="A143" s="26" t="s">
         <v>598</v>
       </c>
-      <c r="B143" s="27"/>
-      <c r="C143" s="27"/>
+      <c r="B143" s="18" t="s">
+        <v>1044</v>
+      </c>
+      <c r="C143" s="18" t="s">
+        <v>1045</v>
+      </c>
+      <c r="D143" s="18" t="s">
+        <v>1046</v>
+      </c>
+      <c r="E143" s="18" t="s">
+        <v>342</v>
+      </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A144" s="26" t="s">
@@ -21307,6 +21884,33 @@
     <row r="159" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A159" s="26" t="s">
         <v>599</v>
+      </c>
+      <c r="B159" s="20" t="s">
+        <v>542</v>
+      </c>
+      <c r="C159" s="20" t="s">
+        <v>752</v>
+      </c>
+      <c r="D159" s="20" t="s">
+        <v>753</v>
+      </c>
+      <c r="E159" s="20" t="s">
+        <v>754</v>
+      </c>
+      <c r="F159" s="20" t="s">
+        <v>755</v>
+      </c>
+      <c r="G159" s="20" t="s">
+        <v>756</v>
+      </c>
+      <c r="H159" s="20" t="s">
+        <v>757</v>
+      </c>
+      <c r="I159" s="20" t="s">
+        <v>758</v>
+      </c>
+      <c r="J159" s="20" t="s">
+        <v>759</v>
       </c>
     </row>
     <row r="160" spans="1:13" x14ac:dyDescent="0.2">
@@ -23683,10 +24287,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBDE6A95-C2F5-4A08-869B-2D219C1ED212}">
-  <dimension ref="A1:A54"/>
+  <dimension ref="A1:A55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A55" sqref="A55"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23696,272 +24300,277 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+      <c r="A1" t="s">
+        <v>1983</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="27" t="s">
         <v>766</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="22" t="s">
         <v>762</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="26" t="s">
         <v>814</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="27" t="s">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="27" t="s">
         <v>773</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="26" t="s">
-        <v>959</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="26" t="s">
-        <v>969</v>
+        <v>959</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="26" t="s">
-        <v>967</v>
+        <v>969</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="26" t="s">
+        <v>967</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="26" t="s">
         <v>1039</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" s="27" t="s">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="27" t="s">
         <v>145</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" s="26" t="s">
-        <v>336</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="26" t="s">
-        <v>958</v>
+        <v>336</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="26" t="s">
-        <v>968</v>
+        <v>958</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="26" t="s">
+        <v>968</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="26" t="s">
         <v>1038</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" s="27" t="s">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" s="27" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" s="26" t="s">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" s="26" t="s">
         <v>1043</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" s="27" t="s">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="27" t="s">
         <v>547</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="26" t="s">
-        <v>960</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="26" t="s">
+        <v>960</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="26" t="s">
         <v>970</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="27" t="s">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="27" t="s">
         <v>767</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="26" t="s">
-        <v>1025</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="26" t="s">
-        <v>961</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="26" t="s">
+        <v>961</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="26" t="s">
         <v>971</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" s="27" t="s">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="27" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" s="26" t="s">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="26" t="s">
         <v>987</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" s="27" t="s">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="27" t="s">
         <v>774</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" s="26" t="s">
-        <v>962</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="26" t="s">
+        <v>962</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="26" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" s="27" t="s">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="27" t="s">
         <v>768</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" s="26" t="s">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" s="26" t="s">
         <v>988</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" s="27" t="s">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" s="27" t="s">
         <v>775</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" s="26" t="s">
-        <v>779</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="26" t="s">
+        <v>779</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="26" t="s">
         <v>972</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="27" t="s">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="27" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="26" t="s">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="26" t="s">
         <v>989</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" s="27" t="s">
-        <v>776</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="27" t="s">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" s="27" t="s">
         <v>769</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" s="26" t="s">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" s="26" t="s">
         <v>990</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" s="27" t="s">
-        <v>777</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="27" t="s">
-        <v>770</v>
+        <v>777</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="27" t="s">
+        <v>770</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" s="27" t="s">
         <v>778</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41" s="26" t="s">
-        <v>964</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="26" t="s">
+        <v>964</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" s="26" t="s">
         <v>973</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43" s="27" t="s">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" s="27" t="s">
         <v>771</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A44" s="26" t="s">
-        <v>965</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" s="26" t="s">
+        <v>965</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" s="26" t="s">
         <v>1040</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A46" s="27" t="s">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" s="27" t="s">
         <v>772</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A47" s="26" t="s">
-        <v>991</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" s="26" t="s">
+        <v>991</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" s="26" t="s">
         <v>1041</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49" s="27" t="s">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" s="27" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50" s="26" t="s">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" s="26" t="s">
         <v>992</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A51" s="27" t="s">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" s="27" t="s">
         <v>146</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52" s="26" t="s">
-        <v>966</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" s="26" t="s">
-        <v>1042</v>
+        <v>966</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" s="26" t="s">
+        <v>1042</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" s="26" t="s">
         <v>1166</v>
       </c>
     </row>

</xml_diff>